<commit_message>
update images and files
</commit_message>
<xml_diff>
--- a/assets/images/testing/testResults.xlsx
+++ b/assets/images/testing/testResults.xlsx
@@ -257,7 +257,7 @@
     </r>
   </si>
   <si>
-    <t>TC07</t>
+    <t>TC007</t>
   </si>
   <si>
     <t>Verify all internal anchor links redirect to the correct places</t>
@@ -302,7 +302,7 @@
     <t>Redirects to LinkedIn in a new window</t>
   </si>
   <si>
-    <t>TC08</t>
+    <t>TC008</t>
   </si>
   <si>
     <t>Verify home/landing contains all relevant content and functionality as per design.</t>
@@ -389,7 +389,7 @@
     <t>Email Received</t>
   </si>
   <si>
-    <t>TC09</t>
+    <t>TC009</t>
   </si>
   <si>
     <t>Verify Game contains all relevant content and functionality as per design</t>

</xml_diff>

<commit_message>
update test image and xlsx
</commit_message>
<xml_diff>
--- a/assets/images/testing/testResults.xlsx
+++ b/assets/images/testing/testResults.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="111">
   <si>
     <t>Test Execution Report</t>
   </si>
@@ -22,7 +22,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Step #</t>
+    <t xml:space="preserve">Step </t>
   </si>
   <si>
     <t>Step Description</t>
@@ -68,9 +68,6 @@
     <t>Document check returns no errors</t>
   </si>
   <si>
-    <t>The type attribute is unnecessary for JavaScript resources.  Not a major issue.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -78,35 +75,6 @@
         <rFont val="Calibri"/>
       </rPr>
       <t>Copy and Paste the game.html code from the project files in the direct input tab and click Check.</t>
-    </r>
-  </si>
-  <si>
-    <t>Document check returns 1 error</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>The type attribute is unnecessary for JavaScript resources.  Not a major issue. Also «Bad value for attribute </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>src</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> on element omg: Must be non-empty». The image gets taken from javaScript so not a major issue. </t>
     </r>
   </si>
   <si>
@@ -511,7 +479,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -549,11 +517,6 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Courier"/>
     </font>
   </fonts>
   <fills count="8">
@@ -774,8 +737,8 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1965,40 +1928,36 @@
       <c r="G4" t="s" s="8">
         <v>13</v>
       </c>
-      <c r="H4" t="s" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" ht="103.15" customHeight="1">
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" ht="52.7" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="9">
         <v>3</v>
       </c>
       <c r="D5" t="s" s="8">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s" s="8">
         <v>15</v>
       </c>
       <c r="F5" t="s" s="8">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s" s="8">
         <v>13</v>
       </c>
-      <c r="H5" t="s" s="8">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" ht="75" customHeight="1">
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" ht="54.15" customHeight="1">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="9">
         <v>4</v>
       </c>
       <c r="D6" t="s" s="8">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s" s="8">
         <v>15</v>
@@ -2009,9 +1968,7 @@
       <c r="G6" t="s" s="8">
         <v>13</v>
       </c>
-      <c r="H6" t="s" s="8">
-        <v>16</v>
-      </c>
+      <c r="H6" s="8"/>
     </row>
     <row r="7" ht="15.35" customHeight="1">
       <c r="A7" s="11"/>
@@ -2025,22 +1982,22 @@
     </row>
     <row r="8" ht="41.3" customHeight="1">
       <c r="A8" t="s" s="7">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s" s="8">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" s="9">
         <v>1</v>
       </c>
       <c r="D8" t="s" s="8">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s" s="8">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s" s="8">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s" s="8">
         <v>13</v>
@@ -2054,19 +2011,19 @@
         <v>2</v>
       </c>
       <c r="D9" t="s" s="8">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s" s="8">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F9" t="s" s="8">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G9" t="s" s="8">
         <v>13</v>
       </c>
       <c r="H9" t="s" s="8">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" ht="15.35" customHeight="1">
@@ -2081,48 +2038,48 @@
     </row>
     <row r="11" ht="75.15" customHeight="1">
       <c r="A11" t="s" s="7">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s" s="8">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
       </c>
       <c r="D11" t="s" s="8">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s" s="8">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s" s="8">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G11" t="s" s="8">
         <v>13</v>
       </c>
       <c r="H11" s="10"/>
     </row>
-    <row r="12" ht="71.15" customHeight="1">
+    <row r="12" ht="91.45" customHeight="1">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="9">
         <v>2</v>
       </c>
       <c r="D12" t="s" s="8">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s" s="8">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s" s="8">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G12" t="s" s="8">
         <v>13</v>
       </c>
       <c r="H12" t="s" s="14">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" ht="15.35" customHeight="1">
@@ -2137,22 +2094,22 @@
     </row>
     <row r="14" ht="81.3" customHeight="1">
       <c r="A14" t="s" s="7">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s" s="8">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C14" s="9">
         <v>1</v>
       </c>
       <c r="D14" t="s" s="8">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s" s="8">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F14" t="s" s="8">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s" s="8">
         <v>13</v>
@@ -2166,13 +2123,13 @@
         <v>2</v>
       </c>
       <c r="D15" t="s" s="8">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s" s="8">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s" s="8">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G15" t="s" s="8">
         <v>13</v>
@@ -2186,13 +2143,13 @@
         <v>3</v>
       </c>
       <c r="D16" t="s" s="8">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s" s="8">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s" s="8">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G16" t="s" s="8">
         <v>13</v>
@@ -2206,13 +2163,13 @@
         <v>4</v>
       </c>
       <c r="D17" t="s" s="8">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s" s="8">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F17" t="s" s="8">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G17" t="s" s="8">
         <v>13</v>
@@ -2226,13 +2183,13 @@
         <v>5</v>
       </c>
       <c r="D18" t="s" s="8">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E18" t="s" s="8">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F18" t="s" s="8">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G18" t="s" s="8">
         <v>13</v>
@@ -2251,22 +2208,22 @@
     </row>
     <row r="20" ht="77.5" customHeight="1">
       <c r="A20" t="s" s="7">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s" s="8">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C20" s="9">
         <v>1</v>
       </c>
       <c r="D20" t="s" s="8">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s" s="8">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F20" t="s" s="8">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G20" t="s" s="8">
         <v>13</v>
@@ -2280,13 +2237,13 @@
         <v>2</v>
       </c>
       <c r="D21" t="s" s="8">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E21" t="s" s="8">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F21" t="s" s="8">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G21" t="s" s="8">
         <v>13</v>
@@ -2300,13 +2257,13 @@
         <v>3</v>
       </c>
       <c r="D22" t="s" s="8">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E22" t="s" s="8">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F22" t="s" s="8">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G22" t="s" s="8">
         <v>13</v>
@@ -2320,13 +2277,13 @@
         <v>4</v>
       </c>
       <c r="D23" t="s" s="8">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E23" t="s" s="8">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F23" t="s" s="8">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G23" t="s" s="8">
         <v>13</v>
@@ -2345,22 +2302,22 @@
     </row>
     <row r="25" ht="73.05" customHeight="1">
       <c r="A25" t="s" s="7">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s" s="8">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C25" s="9">
         <v>1</v>
       </c>
       <c r="D25" t="s" s="8">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E25" t="s" s="8">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F25" t="s" s="8">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G25" t="s" s="8">
         <v>13</v>
@@ -2374,13 +2331,13 @@
         <v>2</v>
       </c>
       <c r="D26" t="s" s="8">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E26" t="s" s="8">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F26" t="s" s="8">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G26" t="s" s="8">
         <v>13</v>
@@ -2394,13 +2351,13 @@
         <v>3</v>
       </c>
       <c r="D27" t="s" s="8">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E27" t="s" s="8">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F27" t="s" s="8">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G27" t="s" s="8">
         <v>13</v>
@@ -2414,13 +2371,13 @@
         <v>4</v>
       </c>
       <c r="D28" t="s" s="8">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E28" t="s" s="8">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F28" t="s" s="8">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G28" t="s" s="8">
         <v>13</v>
@@ -2439,22 +2396,22 @@
     </row>
     <row r="30" ht="50.25" customHeight="1">
       <c r="A30" t="s" s="7">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s" s="8">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C30" s="9">
         <v>1</v>
       </c>
       <c r="D30" t="s" s="8">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E30" t="s" s="8">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F30" t="s" s="8">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G30" t="s" s="8">
         <v>13</v>
@@ -2468,13 +2425,13 @@
         <v>2</v>
       </c>
       <c r="D31" t="s" s="8">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E31" t="s" s="8">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F31" t="s" s="8">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G31" t="s" s="8">
         <v>13</v>
@@ -2488,13 +2445,13 @@
         <v>3</v>
       </c>
       <c r="D32" t="s" s="8">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E32" t="s" s="8">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F32" t="s" s="8">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G32" t="s" s="8">
         <v>13</v>
@@ -2508,13 +2465,13 @@
         <v>4</v>
       </c>
       <c r="D33" t="s" s="8">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E33" t="s" s="8">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F33" t="s" s="8">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G33" t="s" s="8">
         <v>13</v>
@@ -2533,22 +2490,22 @@
     </row>
     <row r="35" ht="58" customHeight="1">
       <c r="A35" t="s" s="7">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B35" t="s" s="8">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C35" s="9">
         <v>1</v>
       </c>
       <c r="D35" t="s" s="8">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E35" t="s" s="8">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F35" t="s" s="8">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G35" t="s" s="8">
         <v>13</v>
@@ -2562,13 +2519,13 @@
         <v>2</v>
       </c>
       <c r="D36" t="s" s="8">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E36" t="s" s="8">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F36" t="s" s="8">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G36" t="s" s="8">
         <v>13</v>
@@ -2582,13 +2539,13 @@
         <v>3</v>
       </c>
       <c r="D37" t="s" s="16">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E37" t="s" s="8">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F37" t="s" s="8">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G37" t="s" s="8">
         <v>13</v>
@@ -2602,13 +2559,13 @@
         <v>4</v>
       </c>
       <c r="D38" t="s" s="16">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E38" t="s" s="8">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F38" t="s" s="8">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G38" t="s" s="8">
         <v>13</v>
@@ -2622,13 +2579,13 @@
         <v>5</v>
       </c>
       <c r="D39" t="s" s="8">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E39" t="s" s="8">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F39" t="s" s="8">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G39" t="s" s="8">
         <v>13</v>
@@ -2642,13 +2599,13 @@
         <v>6</v>
       </c>
       <c r="D40" t="s" s="8">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E40" t="s" s="8">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F40" t="s" s="8">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G40" t="s" s="8">
         <v>13</v>
@@ -2662,13 +2619,13 @@
         <v>7</v>
       </c>
       <c r="D41" t="s" s="8">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E41" t="s" s="8">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F41" t="s" s="8">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G41" t="s" s="8">
         <v>13</v>
@@ -2682,13 +2639,13 @@
         <v>8</v>
       </c>
       <c r="D42" t="s" s="8">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E42" t="s" s="8">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F42" t="s" s="8">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G42" t="s" s="8">
         <v>13</v>
@@ -2702,13 +2659,13 @@
         <v>9</v>
       </c>
       <c r="D43" t="s" s="8">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E43" t="s" s="8">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F43" t="s" s="8">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G43" t="s" s="8">
         <v>13</v>
@@ -2722,13 +2679,13 @@
         <v>10</v>
       </c>
       <c r="D44" t="s" s="8">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E44" t="s" s="8">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F44" t="s" s="8">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G44" t="s" s="8">
         <v>13</v>
@@ -2742,13 +2699,13 @@
         <v>11</v>
       </c>
       <c r="D45" t="s" s="8">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E45" t="s" s="8">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F45" t="s" s="8">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G45" t="s" s="8">
         <v>13</v>
@@ -2762,13 +2719,13 @@
         <v>12</v>
       </c>
       <c r="D46" t="s" s="16">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E46" t="s" s="8">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F46" t="s" s="8">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G46" t="s" s="8">
         <v>13</v>
@@ -2787,22 +2744,22 @@
     </row>
     <row r="48" ht="66.65" customHeight="1">
       <c r="A48" t="s" s="7">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B48" t="s" s="8">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C48" s="9">
         <v>1</v>
       </c>
       <c r="D48" t="s" s="8">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E48" t="s" s="8">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F48" t="s" s="8">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G48" t="s" s="8">
         <v>13</v>
@@ -2816,13 +2773,13 @@
         <v>2</v>
       </c>
       <c r="D49" t="s" s="8">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E49" t="s" s="8">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F49" t="s" s="8">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G49" t="s" s="8">
         <v>13</v>
@@ -2836,13 +2793,13 @@
         <v>3</v>
       </c>
       <c r="D50" t="s" s="8">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E50" t="s" s="8">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F50" t="s" s="8">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G50" t="s" s="8">
         <v>13</v>
@@ -2856,13 +2813,13 @@
         <v>4</v>
       </c>
       <c r="D51" t="s" s="8">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E51" t="s" s="8">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F51" t="s" s="8">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G51" t="s" s="8">
         <v>13</v>
@@ -2876,13 +2833,13 @@
         <v>5</v>
       </c>
       <c r="D52" t="s" s="8">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E52" t="s" s="8">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F52" t="s" s="8">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G52" t="s" s="8">
         <v>13</v>
@@ -2901,22 +2858,22 @@
     </row>
     <row r="54" ht="64.3" customHeight="1">
       <c r="A54" t="s" s="7">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B54" t="s" s="8">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C54" s="9">
         <v>1</v>
       </c>
       <c r="D54" t="s" s="8">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E54" t="s" s="8">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F54" t="s" s="8">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G54" t="s" s="8">
         <v>13</v>
@@ -2930,13 +2887,13 @@
         <v>2</v>
       </c>
       <c r="D55" t="s" s="8">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E55" t="s" s="8">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F55" t="s" s="8">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G55" t="s" s="8">
         <v>13</v>
@@ -2950,13 +2907,13 @@
         <v>3</v>
       </c>
       <c r="D56" t="s" s="8">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E56" t="s" s="8">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F56" t="s" s="8">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G56" t="s" s="8">
         <v>13</v>
@@ -2970,13 +2927,13 @@
         <v>2</v>
       </c>
       <c r="D57" t="s" s="8">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E57" t="s" s="8">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F57" t="s" s="8">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G57" t="s" s="8">
         <v>13</v>
@@ -2990,13 +2947,13 @@
         <v>3</v>
       </c>
       <c r="D58" t="s" s="8">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E58" t="s" s="8">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F58" t="s" s="8">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G58" t="s" s="8">
         <v>13</v>
@@ -3010,13 +2967,13 @@
         <v>4</v>
       </c>
       <c r="D59" t="s" s="8">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E59" t="s" s="8">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F59" t="s" s="8">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G59" t="s" s="8">
         <v>13</v>
@@ -3030,13 +2987,13 @@
         <v>5</v>
       </c>
       <c r="D60" t="s" s="8">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E60" t="s" s="8">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F60" t="s" s="8">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G60" t="s" s="8">
         <v>13</v>
@@ -3050,13 +3007,13 @@
         <v>6</v>
       </c>
       <c r="D61" t="s" s="8">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E61" t="s" s="8">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F61" t="s" s="8">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G61" t="s" s="8">
         <v>13</v>
@@ -3070,13 +3027,13 @@
         <v>7</v>
       </c>
       <c r="D62" t="s" s="8">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E62" t="s" s="8">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F62" t="s" s="8">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G62" t="s" s="8">
         <v>13</v>
@@ -3090,13 +3047,13 @@
         <v>8</v>
       </c>
       <c r="D63" t="s" s="16">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E63" t="s" s="8">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F63" t="s" s="8">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G63" t="s" s="8">
         <v>13</v>
@@ -3110,13 +3067,13 @@
         <v>9</v>
       </c>
       <c r="D64" t="s" s="16">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E64" t="s" s="8">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F64" t="s" s="8">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G64" t="s" s="8">
         <v>13</v>
@@ -3135,22 +3092,22 @@
     </row>
     <row r="66" ht="73.95" customHeight="1">
       <c r="A66" t="s" s="7">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B66" t="s" s="8">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C66" s="9">
         <v>1</v>
       </c>
       <c r="D66" t="s" s="8">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E66" t="s" s="8">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F66" t="s" s="8">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G66" t="s" s="8">
         <v>13</v>
@@ -3164,13 +3121,13 @@
         <v>2</v>
       </c>
       <c r="D67" t="s" s="8">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E67" t="s" s="8">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F67" t="s" s="8">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G67" t="s" s="8">
         <v>13</v>

</xml_diff>